<commit_message>
Adjust comments for VRESProfiles (-> v0.1.1), add RoR1 to VRES
</commit_message>
<xml_diff>
--- a/data/example/Power_VRESProfiles.xlsx
+++ b/data/example/Power_VRESProfiles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioA" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioB" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ScenarioA" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ScenarioB" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -665,7 +665,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.0</t>
+          <t>v0.1.1</t>
         </is>
       </c>
     </row>
@@ -991,7 +991,7 @@
       </c>
       <c r="G5" s="8" t="inlineStr">
         <is>
-          <t>Capacity factor for each VRES unit at this k</t>
+          <t>Capacity factor at this representative time step k</t>
         </is>
       </c>
       <c r="H5" s="7" t="n"/>
@@ -4807,7 +4807,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.0</t>
+          <t>v0.1.1</t>
         </is>
       </c>
     </row>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="G5" s="8" t="inlineStr">
         <is>
-          <t>Capacity factor for each VRES unit at this k</t>
+          <t>Capacity factor at this representative time step k</t>
         </is>
       </c>
       <c r="H5" s="7" t="n"/>

</xml_diff>